<commit_message>
bach form excel export
</commit_message>
<xml_diff>
--- a/resources/excels/ExportTotalCashIn.xlsx
+++ b/resources/excels/ExportTotalCashIn.xlsx
@@ -1,12 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HocWeb\PHP\Veho\awa\resources\excels\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="vZzWycs7qIF3JHIkOaNlQvw5P67lZ8cZFc7S6jZUQjE="/>
@@ -48,28 +56,31 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="20.0"/>
+      <sz val="20"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
@@ -79,7 +90,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -89,11 +100,21 @@
     </fill>
   </fills>
   <borders count="3">
-    <border/>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -108,41 +129,43 @@
       <bottom style="thin">
         <color rgb="FFCDCDCD"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -332,87 +355,89 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M990"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.71"/>
-    <col customWidth="1" min="2" max="2" width="16.29"/>
-    <col customWidth="1" min="3" max="3" width="13.86"/>
-    <col customWidth="1" min="4" max="13" width="14.29"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="13" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" ht="27" customHeight="1">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1"/>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="5" t="s">
+    <row r="2" spans="1:13" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:13" ht="14.25" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
     </row>
-    <row r="4" ht="14.25" customHeight="1"/>
-    <row r="5" ht="14.25" customHeight="1"/>
-    <row r="6" ht="14.25" customHeight="1"/>
-    <row r="7" ht="14.25" customHeight="1"/>
-    <row r="8" ht="14.25" customHeight="1"/>
-    <row r="9" ht="14.25" customHeight="1"/>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:13" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:13" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:13" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:13" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:13" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:13" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:13" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:13" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:13" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:13" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:13" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:13" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:13" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -1392,9 +1417,7 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:G1"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>